<commit_message>
adicionei a tabela de faturamento diário por loja
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/faturamento_mensal_lojas.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/faturamento_mensal_lojas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="9">
   <si>
     <t>Mês</t>
   </si>
@@ -26,6 +26,21 @@
   </si>
   <si>
     <t>Ano</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>Bibi Cell Mundi</t>
+  </si>
+  <si>
+    <t>Bibi Cell Manauara</t>
+  </si>
+  <si>
+    <t>Bibi Cell Vieiralves</t>
+  </si>
+  <si>
+    <t>Bibi Cell Ponta Negra</t>
   </si>
 </sst>
 </file>
@@ -383,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D251"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +417,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>7</v>
       </c>
@@ -416,8 +434,11 @@
       <c r="D2">
         <v>2018</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>8</v>
       </c>
@@ -430,8 +451,11 @@
       <c r="D3">
         <v>2018</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>9</v>
       </c>
@@ -444,8 +468,11 @@
       <c r="D4">
         <v>2018</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>10</v>
       </c>
@@ -458,8 +485,11 @@
       <c r="D5">
         <v>2018</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>11</v>
       </c>
@@ -472,8 +502,11 @@
       <c r="D6">
         <v>2018</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>12</v>
       </c>
@@ -486,8 +519,11 @@
       <c r="D7">
         <v>2018</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -500,8 +536,11 @@
       <c r="D8">
         <v>2019</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>2</v>
       </c>
@@ -514,8 +553,11 @@
       <c r="D9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>3</v>
       </c>
@@ -528,8 +570,11 @@
       <c r="D10">
         <v>2019</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>4</v>
       </c>
@@ -542,8 +587,11 @@
       <c r="D11">
         <v>2019</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>5</v>
       </c>
@@ -556,8 +604,11 @@
       <c r="D12">
         <v>2019</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>6</v>
       </c>
@@ -570,8 +621,11 @@
       <c r="D13">
         <v>2019</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>7</v>
       </c>
@@ -584,8 +638,11 @@
       <c r="D14">
         <v>2019</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>7</v>
       </c>
@@ -598,8 +655,11 @@
       <c r="D15">
         <v>2019</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>8</v>
       </c>
@@ -612,8 +672,11 @@
       <c r="D16">
         <v>2019</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>8</v>
       </c>
@@ -626,8 +689,11 @@
       <c r="D17">
         <v>2019</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>9</v>
       </c>
@@ -640,8 +706,11 @@
       <c r="D18">
         <v>2019</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>9</v>
       </c>
@@ -654,8 +723,11 @@
       <c r="D19">
         <v>2019</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>9</v>
       </c>
@@ -668,8 +740,11 @@
       <c r="D20">
         <v>2019</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>10</v>
       </c>
@@ -682,8 +757,11 @@
       <c r="D21">
         <v>2019</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>10</v>
       </c>
@@ -696,8 +774,11 @@
       <c r="D22">
         <v>2019</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>10</v>
       </c>
@@ -710,8 +791,11 @@
       <c r="D23">
         <v>2019</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>11</v>
       </c>
@@ -724,8 +808,11 @@
       <c r="D24">
         <v>2019</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>11</v>
       </c>
@@ -738,8 +825,11 @@
       <c r="D25">
         <v>2019</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>11</v>
       </c>
@@ -752,8 +842,11 @@
       <c r="D26">
         <v>2019</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>12</v>
       </c>
@@ -766,8 +859,11 @@
       <c r="D27">
         <v>2019</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>12</v>
       </c>
@@ -780,8 +876,11 @@
       <c r="D28">
         <v>2019</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>12</v>
       </c>
@@ -794,8 +893,11 @@
       <c r="D29">
         <v>2019</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>1</v>
       </c>
@@ -808,8 +910,11 @@
       <c r="D30">
         <v>2020</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>1</v>
       </c>
@@ -822,8 +927,11 @@
       <c r="D31">
         <v>2020</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>1</v>
       </c>
@@ -836,8 +944,11 @@
       <c r="D32">
         <v>2020</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>2</v>
       </c>
@@ -850,8 +961,11 @@
       <c r="D33">
         <v>2020</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>2</v>
       </c>
@@ -864,8 +978,11 @@
       <c r="D34">
         <v>2020</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>2</v>
       </c>
@@ -878,8 +995,11 @@
       <c r="D35">
         <v>2020</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>3</v>
       </c>
@@ -892,8 +1012,11 @@
       <c r="D36">
         <v>2020</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>3</v>
       </c>
@@ -906,8 +1029,11 @@
       <c r="D37">
         <v>2020</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>3</v>
       </c>
@@ -920,8 +1046,11 @@
       <c r="D38">
         <v>2020</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>4</v>
       </c>
@@ -934,8 +1063,11 @@
       <c r="D39">
         <v>2020</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>4</v>
       </c>
@@ -948,8 +1080,11 @@
       <c r="D40">
         <v>2020</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>5</v>
       </c>
@@ -962,8 +1097,11 @@
       <c r="D41">
         <v>2020</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>5</v>
       </c>
@@ -976,8 +1114,11 @@
       <c r="D42">
         <v>2020</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>6</v>
       </c>
@@ -990,8 +1131,11 @@
       <c r="D43">
         <v>2020</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>6</v>
       </c>
@@ -1004,8 +1148,11 @@
       <c r="D44">
         <v>2020</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>6</v>
       </c>
@@ -1018,8 +1165,11 @@
       <c r="D45">
         <v>2020</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>7</v>
       </c>
@@ -1032,8 +1182,11 @@
       <c r="D46">
         <v>2020</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>7</v>
       </c>
@@ -1046,8 +1199,11 @@
       <c r="D47">
         <v>2020</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>7</v>
       </c>
@@ -1060,8 +1216,11 @@
       <c r="D48">
         <v>2020</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>8</v>
       </c>
@@ -1074,8 +1233,11 @@
       <c r="D49">
         <v>2020</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>8</v>
       </c>
@@ -1088,8 +1250,11 @@
       <c r="D50">
         <v>2020</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>8</v>
       </c>
@@ -1102,8 +1267,11 @@
       <c r="D51">
         <v>2020</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>9</v>
       </c>
@@ -1116,8 +1284,11 @@
       <c r="D52">
         <v>2020</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>9</v>
       </c>
@@ -1130,8 +1301,11 @@
       <c r="D53">
         <v>2020</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>9</v>
       </c>
@@ -1144,8 +1318,11 @@
       <c r="D54">
         <v>2020</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>10</v>
       </c>
@@ -1158,8 +1335,11 @@
       <c r="D55">
         <v>2020</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>10</v>
       </c>
@@ -1172,8 +1352,11 @@
       <c r="D56">
         <v>2020</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>10</v>
       </c>
@@ -1186,8 +1369,11 @@
       <c r="D57">
         <v>2020</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>11</v>
       </c>
@@ -1200,8 +1386,11 @@
       <c r="D58">
         <v>2020</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>11</v>
       </c>
@@ -1214,8 +1403,11 @@
       <c r="D59">
         <v>2020</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>11</v>
       </c>
@@ -1228,8 +1420,11 @@
       <c r="D60">
         <v>2020</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>12</v>
       </c>
@@ -1242,8 +1437,11 @@
       <c r="D61">
         <v>2020</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>12</v>
       </c>
@@ -1256,8 +1454,11 @@
       <c r="D62">
         <v>2020</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>12</v>
       </c>
@@ -1270,8 +1471,11 @@
       <c r="D63">
         <v>2020</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>1</v>
       </c>
@@ -1284,8 +1488,11 @@
       <c r="D64">
         <v>2021</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>1</v>
       </c>
@@ -1298,8 +1505,11 @@
       <c r="D65">
         <v>2021</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>2</v>
       </c>
@@ -1312,8 +1522,11 @@
       <c r="D66">
         <v>2021</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>2</v>
       </c>
@@ -1326,8 +1539,11 @@
       <c r="D67">
         <v>2021</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>2</v>
       </c>
@@ -1340,8 +1556,11 @@
       <c r="D68">
         <v>2021</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>3</v>
       </c>
@@ -1354,8 +1573,11 @@
       <c r="D69">
         <v>2021</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>3</v>
       </c>
@@ -1368,8 +1590,11 @@
       <c r="D70">
         <v>2021</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>3</v>
       </c>
@@ -1382,8 +1607,11 @@
       <c r="D71">
         <v>2021</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>4</v>
       </c>
@@ -1396,8 +1624,11 @@
       <c r="D72">
         <v>2021</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>4</v>
       </c>
@@ -1410,8 +1641,11 @@
       <c r="D73">
         <v>2021</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>4</v>
       </c>
@@ -1424,8 +1658,11 @@
       <c r="D74">
         <v>2021</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>5</v>
       </c>
@@ -1438,8 +1675,11 @@
       <c r="D75">
         <v>2021</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>5</v>
       </c>
@@ -1452,8 +1692,11 @@
       <c r="D76">
         <v>2021</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>5</v>
       </c>
@@ -1466,8 +1709,11 @@
       <c r="D77">
         <v>2021</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>6</v>
       </c>
@@ -1480,8 +1726,11 @@
       <c r="D78">
         <v>2021</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>6</v>
       </c>
@@ -1494,8 +1743,11 @@
       <c r="D79">
         <v>2021</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>6</v>
       </c>
@@ -1508,8 +1760,11 @@
       <c r="D80">
         <v>2021</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>7</v>
       </c>
@@ -1522,8 +1777,11 @@
       <c r="D81">
         <v>2021</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>7</v>
       </c>
@@ -1536,8 +1794,11 @@
       <c r="D82">
         <v>2021</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>7</v>
       </c>
@@ -1550,8 +1811,11 @@
       <c r="D83">
         <v>2021</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>8</v>
       </c>
@@ -1564,8 +1828,11 @@
       <c r="D84">
         <v>2021</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>8</v>
       </c>
@@ -1578,8 +1845,11 @@
       <c r="D85">
         <v>2021</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>8</v>
       </c>
@@ -1592,8 +1862,11 @@
       <c r="D86">
         <v>2021</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>9</v>
       </c>
@@ -1606,8 +1879,11 @@
       <c r="D87">
         <v>2021</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>9</v>
       </c>
@@ -1620,8 +1896,11 @@
       <c r="D88">
         <v>2021</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>9</v>
       </c>
@@ -1634,8 +1913,11 @@
       <c r="D89">
         <v>2021</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>10</v>
       </c>
@@ -1648,8 +1930,11 @@
       <c r="D90">
         <v>2021</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>10</v>
       </c>
@@ -1662,8 +1947,11 @@
       <c r="D91">
         <v>2021</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>10</v>
       </c>
@@ -1676,8 +1964,11 @@
       <c r="D92">
         <v>2021</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>11</v>
       </c>
@@ -1690,8 +1981,11 @@
       <c r="D93">
         <v>2021</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>11</v>
       </c>
@@ -1704,8 +1998,11 @@
       <c r="D94">
         <v>2021</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>11</v>
       </c>
@@ -1718,8 +2015,11 @@
       <c r="D95">
         <v>2021</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>12</v>
       </c>
@@ -1732,8 +2032,11 @@
       <c r="D96">
         <v>2021</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>12</v>
       </c>
@@ -1746,8 +2049,11 @@
       <c r="D97">
         <v>2021</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>12</v>
       </c>
@@ -1760,8 +2066,11 @@
       <c r="D98">
         <v>2021</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>1</v>
       </c>
@@ -1774,8 +2083,11 @@
       <c r="D99">
         <v>2022</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>1</v>
       </c>
@@ -1788,8 +2100,11 @@
       <c r="D100">
         <v>2022</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="E100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>1</v>
       </c>
@@ -1802,8 +2117,11 @@
       <c r="D101">
         <v>2022</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>2</v>
       </c>
@@ -1816,8 +2134,11 @@
       <c r="D102">
         <v>2022</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>2</v>
       </c>
@@ -1830,8 +2151,11 @@
       <c r="D103">
         <v>2022</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>2</v>
       </c>
@@ -1844,8 +2168,11 @@
       <c r="D104">
         <v>2022</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="E104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>3</v>
       </c>
@@ -1858,8 +2185,11 @@
       <c r="D105">
         <v>2022</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="E105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>3</v>
       </c>
@@ -1872,8 +2202,11 @@
       <c r="D106">
         <v>2022</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="E106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>3</v>
       </c>
@@ -1886,8 +2219,11 @@
       <c r="D107">
         <v>2022</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="E107" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>4</v>
       </c>
@@ -1900,8 +2236,11 @@
       <c r="D108">
         <v>2022</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="E108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>4</v>
       </c>
@@ -1914,8 +2253,11 @@
       <c r="D109">
         <v>2022</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="E109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>4</v>
       </c>
@@ -1928,8 +2270,11 @@
       <c r="D110">
         <v>2022</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="E110" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>5</v>
       </c>
@@ -1942,8 +2287,11 @@
       <c r="D111">
         <v>2022</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="E111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>5</v>
       </c>
@@ -1956,8 +2304,11 @@
       <c r="D112">
         <v>2022</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>5</v>
       </c>
@@ -1970,8 +2321,11 @@
       <c r="D113">
         <v>2022</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="E113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114">
         <v>6</v>
       </c>
@@ -1984,8 +2338,11 @@
       <c r="D114">
         <v>2022</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="E114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115">
         <v>6</v>
       </c>
@@ -1998,8 +2355,11 @@
       <c r="D115">
         <v>2022</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="E115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116">
         <v>6</v>
       </c>
@@ -2012,8 +2372,11 @@
       <c r="D116">
         <v>2022</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="E116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117">
         <v>7</v>
       </c>
@@ -2026,8 +2389,11 @@
       <c r="D117">
         <v>2022</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="E117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118">
         <v>7</v>
       </c>
@@ -2040,8 +2406,11 @@
       <c r="D118">
         <v>2022</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="E118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119">
         <v>7</v>
       </c>
@@ -2054,8 +2423,11 @@
       <c r="D119">
         <v>2022</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120">
         <v>8</v>
       </c>
@@ -2068,8 +2440,11 @@
       <c r="D120">
         <v>2022</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="E120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121">
         <v>8</v>
       </c>
@@ -2082,8 +2457,11 @@
       <c r="D121">
         <v>2022</v>
       </c>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="E121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122">
         <v>8</v>
       </c>
@@ -2096,8 +2474,11 @@
       <c r="D122">
         <v>2022</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="E122" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123">
         <v>8</v>
       </c>
@@ -2110,8 +2491,11 @@
       <c r="D123">
         <v>2022</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="E123" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124">
         <v>9</v>
       </c>
@@ -2124,8 +2508,11 @@
       <c r="D124">
         <v>2022</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="E124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125">
         <v>9</v>
       </c>
@@ -2138,8 +2525,11 @@
       <c r="D125">
         <v>2022</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="E125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126">
         <v>9</v>
       </c>
@@ -2152,8 +2542,11 @@
       <c r="D126">
         <v>2022</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="E126" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127">
         <v>9</v>
       </c>
@@ -2166,8 +2559,11 @@
       <c r="D127">
         <v>2022</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="E127" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128">
         <v>10</v>
       </c>
@@ -2180,8 +2576,11 @@
       <c r="D128">
         <v>2022</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129">
         <v>10</v>
       </c>
@@ -2194,8 +2593,11 @@
       <c r="D129">
         <v>2022</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="E129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130">
         <v>10</v>
       </c>
@@ -2208,8 +2610,11 @@
       <c r="D130">
         <v>2022</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131">
         <v>10</v>
       </c>
@@ -2222,8 +2627,11 @@
       <c r="D131">
         <v>2022</v>
       </c>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="E131" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132">
         <v>11</v>
       </c>
@@ -2236,8 +2644,11 @@
       <c r="D132">
         <v>2022</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="E132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133">
         <v>11</v>
       </c>
@@ -2250,8 +2661,11 @@
       <c r="D133">
         <v>2022</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134">
         <v>11</v>
       </c>
@@ -2264,8 +2678,11 @@
       <c r="D134">
         <v>2022</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="E134" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135">
         <v>11</v>
       </c>
@@ -2278,8 +2695,11 @@
       <c r="D135">
         <v>2022</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="E135" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136">
         <v>12</v>
       </c>
@@ -2292,8 +2712,11 @@
       <c r="D136">
         <v>2022</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="E136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137">
         <v>12</v>
       </c>
@@ -2306,8 +2729,11 @@
       <c r="D137">
         <v>2022</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="E137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138">
         <v>12</v>
       </c>
@@ -2320,8 +2746,11 @@
       <c r="D138">
         <v>2022</v>
       </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="E138" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139">
         <v>12</v>
       </c>
@@ -2334,8 +2763,11 @@
       <c r="D139">
         <v>2022</v>
       </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="E139" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140">
         <v>1</v>
       </c>
@@ -2348,8 +2780,11 @@
       <c r="D140">
         <v>2023</v>
       </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="E140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141">
         <v>1</v>
       </c>
@@ -2362,8 +2797,11 @@
       <c r="D141">
         <v>2023</v>
       </c>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="E141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142">
         <v>1</v>
       </c>
@@ -2376,8 +2814,11 @@
       <c r="D142">
         <v>2023</v>
       </c>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="E142" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143">
         <v>1</v>
       </c>
@@ -2390,8 +2831,11 @@
       <c r="D143">
         <v>2023</v>
       </c>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="E143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144">
         <v>2</v>
       </c>
@@ -2404,8 +2848,11 @@
       <c r="D144">
         <v>2023</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="E144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145">
         <v>2</v>
       </c>
@@ -2418,8 +2865,11 @@
       <c r="D145">
         <v>2023</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="E145" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146">
         <v>2</v>
       </c>
@@ -2432,8 +2882,11 @@
       <c r="D146">
         <v>2023</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="E146" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147">
         <v>2</v>
       </c>
@@ -2446,8 +2899,11 @@
       <c r="D147">
         <v>2023</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="E147" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148">
         <v>3</v>
       </c>
@@ -2460,8 +2916,11 @@
       <c r="D148">
         <v>2023</v>
       </c>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="E148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149">
         <v>3</v>
       </c>
@@ -2474,8 +2933,11 @@
       <c r="D149">
         <v>2023</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="E149" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150">
         <v>3</v>
       </c>
@@ -2488,8 +2950,11 @@
       <c r="D150">
         <v>2023</v>
       </c>
-    </row>
-    <row r="151" spans="1:4">
+      <c r="E150" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151">
         <v>3</v>
       </c>
@@ -2502,8 +2967,11 @@
       <c r="D151">
         <v>2023</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="E151" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152">
         <v>4</v>
       </c>
@@ -2516,8 +2984,11 @@
       <c r="D152">
         <v>2023</v>
       </c>
-    </row>
-    <row r="153" spans="1:4">
+      <c r="E152" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153">
         <v>4</v>
       </c>
@@ -2530,8 +3001,11 @@
       <c r="D153">
         <v>2023</v>
       </c>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="E153" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154">
         <v>4</v>
       </c>
@@ -2544,8 +3018,11 @@
       <c r="D154">
         <v>2023</v>
       </c>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="E154" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155">
         <v>4</v>
       </c>
@@ -2558,8 +3035,11 @@
       <c r="D155">
         <v>2023</v>
       </c>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="E155" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
       <c r="A156">
         <v>5</v>
       </c>
@@ -2572,8 +3052,11 @@
       <c r="D156">
         <v>2023</v>
       </c>
-    </row>
-    <row r="157" spans="1:4">
+      <c r="E156" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
       <c r="A157">
         <v>5</v>
       </c>
@@ -2586,8 +3069,11 @@
       <c r="D157">
         <v>2023</v>
       </c>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="E157" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
       <c r="A158">
         <v>5</v>
       </c>
@@ -2600,8 +3086,11 @@
       <c r="D158">
         <v>2023</v>
       </c>
-    </row>
-    <row r="159" spans="1:4">
+      <c r="E158" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
       <c r="A159">
         <v>5</v>
       </c>
@@ -2614,8 +3103,11 @@
       <c r="D159">
         <v>2023</v>
       </c>
-    </row>
-    <row r="160" spans="1:4">
+      <c r="E159" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
       <c r="A160">
         <v>6</v>
       </c>
@@ -2628,8 +3120,11 @@
       <c r="D160">
         <v>2023</v>
       </c>
-    </row>
-    <row r="161" spans="1:4">
+      <c r="E160" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
       <c r="A161">
         <v>6</v>
       </c>
@@ -2642,8 +3137,11 @@
       <c r="D161">
         <v>2023</v>
       </c>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="E161" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162">
         <v>6</v>
       </c>
@@ -2656,8 +3154,11 @@
       <c r="D162">
         <v>2023</v>
       </c>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="E162" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163">
         <v>6</v>
       </c>
@@ -2670,8 +3171,11 @@
       <c r="D163">
         <v>2023</v>
       </c>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="E163" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164">
         <v>7</v>
       </c>
@@ -2684,8 +3188,11 @@
       <c r="D164">
         <v>2023</v>
       </c>
-    </row>
-    <row r="165" spans="1:4">
+      <c r="E164" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
       <c r="A165">
         <v>7</v>
       </c>
@@ -2698,8 +3205,11 @@
       <c r="D165">
         <v>2023</v>
       </c>
-    </row>
-    <row r="166" spans="1:4">
+      <c r="E165" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166">
         <v>7</v>
       </c>
@@ -2712,8 +3222,11 @@
       <c r="D166">
         <v>2023</v>
       </c>
-    </row>
-    <row r="167" spans="1:4">
+      <c r="E166" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
       <c r="A167">
         <v>7</v>
       </c>
@@ -2726,8 +3239,11 @@
       <c r="D167">
         <v>2023</v>
       </c>
-    </row>
-    <row r="168" spans="1:4">
+      <c r="E167" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
       <c r="A168">
         <v>8</v>
       </c>
@@ -2740,8 +3256,11 @@
       <c r="D168">
         <v>2023</v>
       </c>
-    </row>
-    <row r="169" spans="1:4">
+      <c r="E168" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
       <c r="A169">
         <v>8</v>
       </c>
@@ -2754,8 +3273,11 @@
       <c r="D169">
         <v>2023</v>
       </c>
-    </row>
-    <row r="170" spans="1:4">
+      <c r="E169" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170">
         <v>8</v>
       </c>
@@ -2768,8 +3290,11 @@
       <c r="D170">
         <v>2023</v>
       </c>
-    </row>
-    <row r="171" spans="1:4">
+      <c r="E170" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
       <c r="A171">
         <v>8</v>
       </c>
@@ -2782,8 +3307,11 @@
       <c r="D171">
         <v>2023</v>
       </c>
-    </row>
-    <row r="172" spans="1:4">
+      <c r="E171" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172">
         <v>9</v>
       </c>
@@ -2796,8 +3324,11 @@
       <c r="D172">
         <v>2023</v>
       </c>
-    </row>
-    <row r="173" spans="1:4">
+      <c r="E172" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
       <c r="A173">
         <v>9</v>
       </c>
@@ -2810,8 +3341,11 @@
       <c r="D173">
         <v>2023</v>
       </c>
-    </row>
-    <row r="174" spans="1:4">
+      <c r="E173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
       <c r="A174">
         <v>9</v>
       </c>
@@ -2824,8 +3358,11 @@
       <c r="D174">
         <v>2023</v>
       </c>
-    </row>
-    <row r="175" spans="1:4">
+      <c r="E174" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
       <c r="A175">
         <v>9</v>
       </c>
@@ -2838,8 +3375,11 @@
       <c r="D175">
         <v>2023</v>
       </c>
-    </row>
-    <row r="176" spans="1:4">
+      <c r="E175" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
       <c r="A176">
         <v>10</v>
       </c>
@@ -2852,8 +3392,11 @@
       <c r="D176">
         <v>2023</v>
       </c>
-    </row>
-    <row r="177" spans="1:4">
+      <c r="E176" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
       <c r="A177">
         <v>10</v>
       </c>
@@ -2866,8 +3409,11 @@
       <c r="D177">
         <v>2023</v>
       </c>
-    </row>
-    <row r="178" spans="1:4">
+      <c r="E177" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
       <c r="A178">
         <v>10</v>
       </c>
@@ -2880,8 +3426,11 @@
       <c r="D178">
         <v>2023</v>
       </c>
-    </row>
-    <row r="179" spans="1:4">
+      <c r="E178" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
       <c r="A179">
         <v>10</v>
       </c>
@@ -2894,8 +3443,11 @@
       <c r="D179">
         <v>2023</v>
       </c>
-    </row>
-    <row r="180" spans="1:4">
+      <c r="E179" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
       <c r="A180">
         <v>11</v>
       </c>
@@ -2908,8 +3460,11 @@
       <c r="D180">
         <v>2023</v>
       </c>
-    </row>
-    <row r="181" spans="1:4">
+      <c r="E180" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
       <c r="A181">
         <v>11</v>
       </c>
@@ -2922,8 +3477,11 @@
       <c r="D181">
         <v>2023</v>
       </c>
-    </row>
-    <row r="182" spans="1:4">
+      <c r="E181" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
       <c r="A182">
         <v>11</v>
       </c>
@@ -2936,8 +3494,11 @@
       <c r="D182">
         <v>2023</v>
       </c>
-    </row>
-    <row r="183" spans="1:4">
+      <c r="E182" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
       <c r="A183">
         <v>11</v>
       </c>
@@ -2950,8 +3511,11 @@
       <c r="D183">
         <v>2023</v>
       </c>
-    </row>
-    <row r="184" spans="1:4">
+      <c r="E183" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
       <c r="A184">
         <v>12</v>
       </c>
@@ -2964,8 +3528,11 @@
       <c r="D184">
         <v>2023</v>
       </c>
-    </row>
-    <row r="185" spans="1:4">
+      <c r="E184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
       <c r="A185">
         <v>12</v>
       </c>
@@ -2978,8 +3545,11 @@
       <c r="D185">
         <v>2023</v>
       </c>
-    </row>
-    <row r="186" spans="1:4">
+      <c r="E185" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
       <c r="A186">
         <v>12</v>
       </c>
@@ -2992,8 +3562,11 @@
       <c r="D186">
         <v>2023</v>
       </c>
-    </row>
-    <row r="187" spans="1:4">
+      <c r="E186" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
       <c r="A187">
         <v>12</v>
       </c>
@@ -3006,8 +3579,11 @@
       <c r="D187">
         <v>2023</v>
       </c>
-    </row>
-    <row r="188" spans="1:4">
+      <c r="E187" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
       <c r="A188">
         <v>1</v>
       </c>
@@ -3020,8 +3596,11 @@
       <c r="D188">
         <v>2024</v>
       </c>
-    </row>
-    <row r="189" spans="1:4">
+      <c r="E188" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
       <c r="A189">
         <v>1</v>
       </c>
@@ -3034,8 +3613,11 @@
       <c r="D189">
         <v>2024</v>
       </c>
-    </row>
-    <row r="190" spans="1:4">
+      <c r="E189" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
       <c r="A190">
         <v>1</v>
       </c>
@@ -3048,8 +3630,11 @@
       <c r="D190">
         <v>2024</v>
       </c>
-    </row>
-    <row r="191" spans="1:4">
+      <c r="E190" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
       <c r="A191">
         <v>1</v>
       </c>
@@ -3062,8 +3647,11 @@
       <c r="D191">
         <v>2024</v>
       </c>
-    </row>
-    <row r="192" spans="1:4">
+      <c r="E191" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
       <c r="A192">
         <v>2</v>
       </c>
@@ -3076,8 +3664,11 @@
       <c r="D192">
         <v>2024</v>
       </c>
-    </row>
-    <row r="193" spans="1:4">
+      <c r="E192" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
       <c r="A193">
         <v>2</v>
       </c>
@@ -3090,8 +3681,11 @@
       <c r="D193">
         <v>2024</v>
       </c>
-    </row>
-    <row r="194" spans="1:4">
+      <c r="E193" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
       <c r="A194">
         <v>2</v>
       </c>
@@ -3104,8 +3698,11 @@
       <c r="D194">
         <v>2024</v>
       </c>
-    </row>
-    <row r="195" spans="1:4">
+      <c r="E194" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
       <c r="A195">
         <v>2</v>
       </c>
@@ -3118,8 +3715,11 @@
       <c r="D195">
         <v>2024</v>
       </c>
-    </row>
-    <row r="196" spans="1:4">
+      <c r="E195" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
       <c r="A196">
         <v>3</v>
       </c>
@@ -3132,8 +3732,11 @@
       <c r="D196">
         <v>2024</v>
       </c>
-    </row>
-    <row r="197" spans="1:4">
+      <c r="E196" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
       <c r="A197">
         <v>3</v>
       </c>
@@ -3146,8 +3749,11 @@
       <c r="D197">
         <v>2024</v>
       </c>
-    </row>
-    <row r="198" spans="1:4">
+      <c r="E197" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
       <c r="A198">
         <v>3</v>
       </c>
@@ -3160,8 +3766,11 @@
       <c r="D198">
         <v>2024</v>
       </c>
-    </row>
-    <row r="199" spans="1:4">
+      <c r="E198" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
       <c r="A199">
         <v>3</v>
       </c>
@@ -3174,8 +3783,11 @@
       <c r="D199">
         <v>2024</v>
       </c>
-    </row>
-    <row r="200" spans="1:4">
+      <c r="E199" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
       <c r="A200">
         <v>4</v>
       </c>
@@ -3188,8 +3800,11 @@
       <c r="D200">
         <v>2024</v>
       </c>
-    </row>
-    <row r="201" spans="1:4">
+      <c r="E200" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
       <c r="A201">
         <v>4</v>
       </c>
@@ -3202,8 +3817,11 @@
       <c r="D201">
         <v>2024</v>
       </c>
-    </row>
-    <row r="202" spans="1:4">
+      <c r="E201" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
       <c r="A202">
         <v>4</v>
       </c>
@@ -3216,8 +3834,11 @@
       <c r="D202">
         <v>2024</v>
       </c>
-    </row>
-    <row r="203" spans="1:4">
+      <c r="E202" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
       <c r="A203">
         <v>4</v>
       </c>
@@ -3230,8 +3851,11 @@
       <c r="D203">
         <v>2024</v>
       </c>
-    </row>
-    <row r="204" spans="1:4">
+      <c r="E203" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
       <c r="A204">
         <v>5</v>
       </c>
@@ -3244,8 +3868,11 @@
       <c r="D204">
         <v>2024</v>
       </c>
-    </row>
-    <row r="205" spans="1:4">
+      <c r="E204" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
       <c r="A205">
         <v>5</v>
       </c>
@@ -3258,8 +3885,11 @@
       <c r="D205">
         <v>2024</v>
       </c>
-    </row>
-    <row r="206" spans="1:4">
+      <c r="E205" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
       <c r="A206">
         <v>5</v>
       </c>
@@ -3272,8 +3902,11 @@
       <c r="D206">
         <v>2024</v>
       </c>
-    </row>
-    <row r="207" spans="1:4">
+      <c r="E206" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
       <c r="A207">
         <v>5</v>
       </c>
@@ -3286,8 +3919,11 @@
       <c r="D207">
         <v>2024</v>
       </c>
-    </row>
-    <row r="208" spans="1:4">
+      <c r="E207" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
       <c r="A208">
         <v>6</v>
       </c>
@@ -3300,8 +3936,11 @@
       <c r="D208">
         <v>2024</v>
       </c>
-    </row>
-    <row r="209" spans="1:4">
+      <c r="E208" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
       <c r="A209">
         <v>6</v>
       </c>
@@ -3314,8 +3953,11 @@
       <c r="D209">
         <v>2024</v>
       </c>
-    </row>
-    <row r="210" spans="1:4">
+      <c r="E209" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
       <c r="A210">
         <v>6</v>
       </c>
@@ -3328,8 +3970,11 @@
       <c r="D210">
         <v>2024</v>
       </c>
-    </row>
-    <row r="211" spans="1:4">
+      <c r="E210" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
       <c r="A211">
         <v>6</v>
       </c>
@@ -3342,8 +3987,11 @@
       <c r="D211">
         <v>2024</v>
       </c>
-    </row>
-    <row r="212" spans="1:4">
+      <c r="E211" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
       <c r="A212">
         <v>7</v>
       </c>
@@ -3356,8 +4004,11 @@
       <c r="D212">
         <v>2024</v>
       </c>
-    </row>
-    <row r="213" spans="1:4">
+      <c r="E212" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
       <c r="A213">
         <v>7</v>
       </c>
@@ -3370,8 +4021,11 @@
       <c r="D213">
         <v>2024</v>
       </c>
-    </row>
-    <row r="214" spans="1:4">
+      <c r="E213" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
       <c r="A214">
         <v>7</v>
       </c>
@@ -3384,8 +4038,11 @@
       <c r="D214">
         <v>2024</v>
       </c>
-    </row>
-    <row r="215" spans="1:4">
+      <c r="E214" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
       <c r="A215">
         <v>7</v>
       </c>
@@ -3398,8 +4055,11 @@
       <c r="D215">
         <v>2024</v>
       </c>
-    </row>
-    <row r="216" spans="1:4">
+      <c r="E215" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
       <c r="A216">
         <v>8</v>
       </c>
@@ -3412,8 +4072,11 @@
       <c r="D216">
         <v>2024</v>
       </c>
-    </row>
-    <row r="217" spans="1:4">
+      <c r="E216" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
       <c r="A217">
         <v>8</v>
       </c>
@@ -3426,8 +4089,11 @@
       <c r="D217">
         <v>2024</v>
       </c>
-    </row>
-    <row r="218" spans="1:4">
+      <c r="E217" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
       <c r="A218">
         <v>8</v>
       </c>
@@ -3440,8 +4106,11 @@
       <c r="D218">
         <v>2024</v>
       </c>
-    </row>
-    <row r="219" spans="1:4">
+      <c r="E218" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
       <c r="A219">
         <v>8</v>
       </c>
@@ -3454,8 +4123,11 @@
       <c r="D219">
         <v>2024</v>
       </c>
-    </row>
-    <row r="220" spans="1:4">
+      <c r="E219" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
       <c r="A220">
         <v>9</v>
       </c>
@@ -3468,8 +4140,11 @@
       <c r="D220">
         <v>2024</v>
       </c>
-    </row>
-    <row r="221" spans="1:4">
+      <c r="E220" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
       <c r="A221">
         <v>9</v>
       </c>
@@ -3482,8 +4157,11 @@
       <c r="D221">
         <v>2024</v>
       </c>
-    </row>
-    <row r="222" spans="1:4">
+      <c r="E221" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
       <c r="A222">
         <v>9</v>
       </c>
@@ -3496,8 +4174,11 @@
       <c r="D222">
         <v>2024</v>
       </c>
-    </row>
-    <row r="223" spans="1:4">
+      <c r="E222" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
       <c r="A223">
         <v>9</v>
       </c>
@@ -3510,8 +4191,11 @@
       <c r="D223">
         <v>2024</v>
       </c>
-    </row>
-    <row r="224" spans="1:4">
+      <c r="E223" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
       <c r="A224">
         <v>10</v>
       </c>
@@ -3524,8 +4208,11 @@
       <c r="D224">
         <v>2024</v>
       </c>
-    </row>
-    <row r="225" spans="1:4">
+      <c r="E224" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
       <c r="A225">
         <v>10</v>
       </c>
@@ -3538,8 +4225,11 @@
       <c r="D225">
         <v>2024</v>
       </c>
-    </row>
-    <row r="226" spans="1:4">
+      <c r="E225" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
       <c r="A226">
         <v>10</v>
       </c>
@@ -3552,8 +4242,11 @@
       <c r="D226">
         <v>2024</v>
       </c>
-    </row>
-    <row r="227" spans="1:4">
+      <c r="E226" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
       <c r="A227">
         <v>10</v>
       </c>
@@ -3566,8 +4259,11 @@
       <c r="D227">
         <v>2024</v>
       </c>
-    </row>
-    <row r="228" spans="1:4">
+      <c r="E227" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
       <c r="A228">
         <v>11</v>
       </c>
@@ -3580,8 +4276,11 @@
       <c r="D228">
         <v>2024</v>
       </c>
-    </row>
-    <row r="229" spans="1:4">
+      <c r="E228" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
       <c r="A229">
         <v>11</v>
       </c>
@@ -3594,8 +4293,11 @@
       <c r="D229">
         <v>2024</v>
       </c>
-    </row>
-    <row r="230" spans="1:4">
+      <c r="E229" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
       <c r="A230">
         <v>11</v>
       </c>
@@ -3608,8 +4310,11 @@
       <c r="D230">
         <v>2024</v>
       </c>
-    </row>
-    <row r="231" spans="1:4">
+      <c r="E230" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
       <c r="A231">
         <v>11</v>
       </c>
@@ -3622,8 +4327,11 @@
       <c r="D231">
         <v>2024</v>
       </c>
-    </row>
-    <row r="232" spans="1:4">
+      <c r="E231" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
       <c r="A232">
         <v>12</v>
       </c>
@@ -3636,8 +4344,11 @@
       <c r="D232">
         <v>2024</v>
       </c>
-    </row>
-    <row r="233" spans="1:4">
+      <c r="E232" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
       <c r="A233">
         <v>12</v>
       </c>
@@ -3650,8 +4361,11 @@
       <c r="D233">
         <v>2024</v>
       </c>
-    </row>
-    <row r="234" spans="1:4">
+      <c r="E233" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
       <c r="A234">
         <v>12</v>
       </c>
@@ -3664,8 +4378,11 @@
       <c r="D234">
         <v>2024</v>
       </c>
-    </row>
-    <row r="235" spans="1:4">
+      <c r="E234" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
       <c r="A235">
         <v>12</v>
       </c>
@@ -3678,8 +4395,11 @@
       <c r="D235">
         <v>2024</v>
       </c>
-    </row>
-    <row r="236" spans="1:4">
+      <c r="E235" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
       <c r="A236">
         <v>1</v>
       </c>
@@ -3692,8 +4412,11 @@
       <c r="D236">
         <v>2025</v>
       </c>
-    </row>
-    <row r="237" spans="1:4">
+      <c r="E236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
       <c r="A237">
         <v>1</v>
       </c>
@@ -3706,8 +4429,11 @@
       <c r="D237">
         <v>2025</v>
       </c>
-    </row>
-    <row r="238" spans="1:4">
+      <c r="E237" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
       <c r="A238">
         <v>1</v>
       </c>
@@ -3720,8 +4446,11 @@
       <c r="D238">
         <v>2025</v>
       </c>
-    </row>
-    <row r="239" spans="1:4">
+      <c r="E238" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
       <c r="A239">
         <v>1</v>
       </c>
@@ -3734,8 +4463,11 @@
       <c r="D239">
         <v>2025</v>
       </c>
-    </row>
-    <row r="240" spans="1:4">
+      <c r="E239" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
       <c r="A240">
         <v>2</v>
       </c>
@@ -3748,8 +4480,11 @@
       <c r="D240">
         <v>2025</v>
       </c>
-    </row>
-    <row r="241" spans="1:4">
+      <c r="E240" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
       <c r="A241">
         <v>2</v>
       </c>
@@ -3762,8 +4497,11 @@
       <c r="D241">
         <v>2025</v>
       </c>
-    </row>
-    <row r="242" spans="1:4">
+      <c r="E241" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
       <c r="A242">
         <v>2</v>
       </c>
@@ -3776,8 +4514,11 @@
       <c r="D242">
         <v>2025</v>
       </c>
-    </row>
-    <row r="243" spans="1:4">
+      <c r="E242" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
       <c r="A243">
         <v>2</v>
       </c>
@@ -3790,8 +4531,11 @@
       <c r="D243">
         <v>2025</v>
       </c>
-    </row>
-    <row r="244" spans="1:4">
+      <c r="E243" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
       <c r="A244">
         <v>3</v>
       </c>
@@ -3804,8 +4548,11 @@
       <c r="D244">
         <v>2025</v>
       </c>
-    </row>
-    <row r="245" spans="1:4">
+      <c r="E244" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
       <c r="A245">
         <v>3</v>
       </c>
@@ -3818,8 +4565,11 @@
       <c r="D245">
         <v>2025</v>
       </c>
-    </row>
-    <row r="246" spans="1:4">
+      <c r="E245" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
       <c r="A246">
         <v>3</v>
       </c>
@@ -3832,8 +4582,11 @@
       <c r="D246">
         <v>2025</v>
       </c>
-    </row>
-    <row r="247" spans="1:4">
+      <c r="E246" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
       <c r="A247">
         <v>3</v>
       </c>
@@ -3846,8 +4599,11 @@
       <c r="D247">
         <v>2025</v>
       </c>
-    </row>
-    <row r="248" spans="1:4">
+      <c r="E247" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
       <c r="A248">
         <v>4</v>
       </c>
@@ -3860,8 +4616,11 @@
       <c r="D248">
         <v>2025</v>
       </c>
-    </row>
-    <row r="249" spans="1:4">
+      <c r="E248" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
       <c r="A249">
         <v>4</v>
       </c>
@@ -3874,8 +4633,11 @@
       <c r="D249">
         <v>2025</v>
       </c>
-    </row>
-    <row r="250" spans="1:4">
+      <c r="E249" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
       <c r="A250">
         <v>4</v>
       </c>
@@ -3888,8 +4650,11 @@
       <c r="D250">
         <v>2025</v>
       </c>
-    </row>
-    <row r="251" spans="1:4">
+      <c r="E250" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
       <c r="A251">
         <v>4</v>
       </c>
@@ -3901,6 +4666,9 @@
       </c>
       <c r="D251">
         <v>2025</v>
+      </c>
+      <c r="E251" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>